<commit_message>
Fix semantic nonsense in questions: Expand KB and fix fallbacks
</commit_message>
<xml_diff>
--- a/outputs/generated_questions.xlsx
+++ b/outputs/generated_questions.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="tags" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -514,7 +515,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Travis Scott</t>
+          <t>Kendrick Lamar</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -533,7 +534,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>101,50,54</t>
         </is>
       </c>
     </row>
@@ -551,7 +552,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Which artist released 'Blinding Lights'?</t>
+          <t>Who performed at the 2021 Super Bowl Halftime Show?</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -566,7 +567,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Drake</t>
+          <t>Justin Bieber</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -580,7 +581,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>10,100,50,54</t>
         </is>
       </c>
     </row>
@@ -608,12 +609,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>J Balvin</t>
+          <t>Maluma</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Maluma</t>
+          <t>Daddy Yankee</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -627,7 +628,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>50,54,99</t>
         </is>
       </c>
     </row>
@@ -645,7 +646,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Which artist started on Nickelodeon's 'Victorious'?</t>
+          <t>Who sings 'thank u, next'?</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -655,12 +656,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Demi Lovato</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>Selena Gomez</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -674,7 +675,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>10,100,101,50,99</t>
         </is>
       </c>
     </row>
@@ -702,12 +703,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Avengers: Endgame</t>
+          <t>Titanic</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Titanic</t>
+          <t>Star Wars</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -721,7 +722,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>10,101,51</t>
         </is>
       </c>
     </row>
@@ -739,7 +740,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Which movie concludes the Infinity Saga?</t>
+          <t>In which movie does Iron Man snap his fingers?</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -754,7 +755,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Civil War</t>
+          <t>Age of Ultron</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -768,7 +769,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>51,54,99</t>
         </is>
       </c>
     </row>
@@ -796,12 +797,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Snapchat</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -815,7 +816,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>100,101,54,7,99</t>
         </is>
       </c>
     </row>
@@ -862,7 +863,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>10,101,99</t>
         </is>
       </c>
     </row>
@@ -909,7 +910,196 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>10,100,101,54,99</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TAG_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TAG_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORY</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>:COUNTRY</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Geography</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>:COMPANY</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ED:HISTORY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EN:MUSIC</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Entertainment</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>EN:MOVIE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Entertainment</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EN:Facts</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NEW:Viral</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Trends</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NEW:Tech</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NEW:Nostalgia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lifestyle</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement Semantic Checker, Multi-Tagging, and Expanded Knowledge Base
</commit_message>
<xml_diff>
--- a/outputs/generated_questions.xlsx
+++ b/outputs/generated_questions.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,7 +505,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Who founded OVO Sound?</t>
+          <t>Which Canadian rapper released 'God's Plan'?</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Kendrick Lamar</t>
+          <t>J. Cole</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -527,14 +527,14 @@
         <v>3013100</v>
       </c>
       <c r="I2" t="n">
-        <v>3013109</v>
+        <v>3013110</v>
       </c>
       <c r="J2" t="n">
-        <v>3013118</v>
+        <v>3013120</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>101,50,54</t>
+          <t>100,50,54,99</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Who performed at the 2021 Super Bowl Halftime Show?</t>
+          <t>Which artist released 'Blinding Lights'?</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -562,26 +562,26 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Bruno Mars</t>
+          <t>Drake</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Justin Bieber</t>
+          <t>Post Malone</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>3013101</v>
       </c>
       <c r="I3" t="n">
-        <v>3013110</v>
+        <v>3013111</v>
       </c>
       <c r="J3" t="n">
-        <v>3013119</v>
+        <v>3013121</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>10,100,50,54</t>
+          <t>10,101,50,54,99</t>
         </is>
       </c>
     </row>
@@ -609,26 +609,26 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Maluma</t>
+          <t>J Balvin</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Daddy Yankee</t>
+          <t>Ozuna</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>3013102</v>
       </c>
       <c r="I4" t="n">
-        <v>3013111</v>
+        <v>3013112</v>
       </c>
       <c r="J4" t="n">
-        <v>3013120</v>
+        <v>3013122</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>50,54,99</t>
+          <t>10,50</t>
         </is>
       </c>
     </row>
@@ -656,26 +656,26 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>Selena Gomez</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Selena Gomez</t>
+          <t>Miley Cyrus</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>3013103</v>
       </c>
       <c r="I5" t="n">
-        <v>3013112</v>
+        <v>3013113</v>
       </c>
       <c r="J5" t="n">
-        <v>3013121</v>
+        <v>3013123</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>10,100,101,50,99</t>
+          <t>101,50,99</t>
         </is>
       </c>
     </row>
@@ -703,7 +703,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Titanic</t>
+          <t>Avengers: Endgame</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -715,14 +715,14 @@
         <v>3013104</v>
       </c>
       <c r="I6" t="n">
-        <v>3013113</v>
+        <v>3013114</v>
       </c>
       <c r="J6" t="n">
-        <v>3013122</v>
+        <v>3013124</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>10,101,51</t>
+          <t>51,54,99</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>In which movie does Iron Man snap his fingers?</t>
+          <t>Which movie concludes the Infinity Saga?</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -750,26 +750,26 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Infinity War</t>
+          <t>Civil War</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Age of Ultron</t>
+          <t>Justice League</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>3013105</v>
       </c>
       <c r="I7" t="n">
-        <v>3013114</v>
+        <v>3013115</v>
       </c>
       <c r="J7" t="n">
-        <v>3013123</v>
+        <v>3013125</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>51,54,99</t>
+          <t>10,101,51</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Which platform was founded by Mark Zuckerberg?</t>
+          <t>Which company owns Instagram and WhatsApp?</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -797,26 +797,26 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>Twitter</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Amazon</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Twitter</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>3013106</v>
       </c>
       <c r="I8" t="n">
-        <v>3013115</v>
+        <v>3013116</v>
       </c>
       <c r="J8" t="n">
-        <v>3013124</v>
+        <v>3013126</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>100,101,54,7,99</t>
+          <t>100,101,7,99</t>
         </is>
       </c>
     </row>
@@ -856,14 +856,14 @@
         <v>3013107</v>
       </c>
       <c r="I9" t="n">
-        <v>3013116</v>
+        <v>3013117</v>
       </c>
       <c r="J9" t="n">
-        <v>3013125</v>
+        <v>3013127</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>10,101,99</t>
+          <t>10,100</t>
         </is>
       </c>
     </row>
@@ -903,14 +903,61 @@
         <v>3013108</v>
       </c>
       <c r="I10" t="n">
-        <v>3013117</v>
+        <v>3013118</v>
       </c>
       <c r="J10" t="n">
-        <v>3013126</v>
+        <v>3013128</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>10,100,101,54,99</t>
+          <t>10,100</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>30140</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Which hormone is associated with stress?</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Cortisol</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Insulin</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Melatonin</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>3013109</v>
+      </c>
+      <c r="I11" t="n">
+        <v>3013119</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3013129</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>10,100,101,54</t>
         </is>
       </c>
     </row>

</xml_diff>